<commit_message>
feat: added dynamic email input to excel resources
</commit_message>
<xml_diff>
--- a/OpenCartAutomation/src/test/resources/InputData.xlsx
+++ b/OpenCartAutomation/src/test/resources/InputData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbf015f5d1ac5c58/Tareas/Semestre 10/QA/QA-Final_Assigment/OpenCartAutomation/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{39843967-FE10-47B1-B092-6964F6F054C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90A74FA9-FE13-49E7-AD35-D0ED08AC4384}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{39843967-FE10-47B1-B092-6964F6F054C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AC68046-410C-4075-AEF8-17C50837FE63}"/>
   <bookViews>
     <workbookView xWindow="1788" yWindow="0" windowWidth="11712" windowHeight="13680" activeTab="1" xr2:uid="{74D3C756-9A7B-440B-B88D-49B4EDD213ED}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>FirstName</t>
   </si>
@@ -79,12 +79,19 @@
   </si>
   <si>
     <t>fail</t>
+  </si>
+  <si>
+    <t>juan.perez99_262@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_840@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,7 +483,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -503,7 +510,7 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>7</v>
       </c>
       <c r="D2" s="1">
@@ -523,25 +530,28 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="38.33203125"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
added test for product search and add to cart
</commit_message>
<xml_diff>
--- a/OpenCartAutomation/src/test/resources/InputData.xlsx
+++ b/OpenCartAutomation/src/test/resources/InputData.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbf015f5d1ac5c58/Tareas/Semestre 10/QA/QA-Final_Assigment/OpenCartAutomation/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{39843967-FE10-47B1-B092-6964F6F054C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AC68046-410C-4075-AEF8-17C50837FE63}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{39843967-FE10-47B1-B092-6964F6F054C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{551EFF07-10D5-4A20-8A09-EC9F907B705A}"/>
   <bookViews>
-    <workbookView xWindow="1788" yWindow="0" windowWidth="11712" windowHeight="13680" activeTab="1" xr2:uid="{74D3C756-9A7B-440B-B88D-49B4EDD213ED}"/>
+    <workbookView minimized="1" xWindow="1788" yWindow="0" windowWidth="11712" windowHeight="13680" firstSheet="1" activeTab="2" xr2:uid="{74D3C756-9A7B-440B-B88D-49B4EDD213ED}"/>
   </bookViews>
   <sheets>
     <sheet name="UsuariosRegistro" sheetId="1" r:id="rId1"/>
     <sheet name="LoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="ProductosBusqueda" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>FirstName</t>
   </si>
@@ -81,18 +82,44 @@
     <t>fail</t>
   </si>
   <si>
-    <t>juan.perez99_262@test.com</t>
-  </si>
-  <si>
     <t>juan.perez99_840@test.com</t>
+  </si>
+  <si>
+    <t>Phones</t>
+  </si>
+  <si>
+    <t>Tablets</t>
+  </si>
+  <si>
+    <t>Cameras</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>SubCategoria</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Tab 10.1</t>
+  </si>
+  <si>
+    <t>Canon EOS 5D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +137,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,10 +171,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -483,7 +519,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.33203125"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -510,7 +546,7 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1">
@@ -529,29 +565,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CC2A3F-D513-4DB3-976A-0E617FE7583C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.33203125"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -577,4 +613,69 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9D6DCA-AA9A-4D49-AD31-3D19F6B898AB}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: added cart vertification test and refactor search test for adding items into cart with logged account
</commit_message>
<xml_diff>
--- a/OpenCartAutomation/src/test/resources/InputData.xlsx
+++ b/OpenCartAutomation/src/test/resources/InputData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbf015f5d1ac5c58/Tareas/Semestre 10/QA/QA-Final_Assigment/OpenCartAutomation/src/test/resources/"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>FirstName</t>
   </si>
@@ -113,12 +113,16 @@
   </si>
   <si>
     <t>Canon EOS 5D</t>
+  </si>
+  <si>
+    <t>juan.perez99_92875@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -519,7 +523,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -546,7 +550,7 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>7</v>
       </c>
       <c r="D2" s="1">
@@ -571,23 +575,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="38.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -626,49 +630,49 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: refactorize pages and utils for matching class description
</commit_message>
<xml_diff>
--- a/OpenCartAutomation/src/test/resources/InputData.xlsx
+++ b/OpenCartAutomation/src/test/resources/InputData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbf015f5d1ac5c58/Tareas/Semestre 10/QA/QA-Final_Assigment/OpenCartAutomation/src/test/resources/"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>FirstName</t>
   </si>
@@ -113,12 +113,28 @@
   </si>
   <si>
     <t>juan.perez99_91364@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_70367@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_31648@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_49537@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_33824@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_20113@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -519,7 +535,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -546,7 +562,7 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>7</v>
       </c>
       <c r="D2" s="1">
@@ -571,23 +587,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="38.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -626,49 +642,49 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: ajdust test order and teardown
</commit_message>
<xml_diff>
--- a/OpenCartAutomation/src/test/resources/InputData.xlsx
+++ b/OpenCartAutomation/src/test/resources/InputData.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>FirstName</t>
   </si>
@@ -112,22 +112,13 @@
     <t>Canon EOS 5D</t>
   </si>
   <si>
-    <t>juan.perez99_91364@test.com</t>
-  </si>
-  <si>
-    <t>juan.perez99_70367@test.com</t>
-  </si>
-  <si>
-    <t>juan.perez99_31648@test.com</t>
-  </si>
-  <si>
-    <t>juan.perez99_49537@test.com</t>
-  </si>
-  <si>
-    <t>juan.perez99_33824@test.com</t>
-  </si>
-  <si>
     <t>juan.perez99_20113@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_20017@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_25911@test.com</t>
   </si>
 </sst>
 </file>
@@ -582,7 +573,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,7 +594,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
fix: delete wait on product page
</commit_message>
<xml_diff>
--- a/OpenCartAutomation/src/test/resources/InputData.xlsx
+++ b/OpenCartAutomation/src/test/resources/InputData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t xml:space="preserve">FirstName</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>juan.perez99_58985@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_74501@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_29683@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_65904@test.com</t>
   </si>
 </sst>
 </file>
@@ -548,7 +557,7 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
have to use console
</commit_message>
<xml_diff>
--- a/OpenCartAutomation/src/test/resources/InputData.xlsx
+++ b/OpenCartAutomation/src/test/resources/InputData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t xml:space="preserve">FirstName</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>juan.perez99_65904@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_68224@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_72264@test.com</t>
+  </si>
+  <si>
+    <t>juan.perez99_46781@test.com</t>
   </si>
 </sst>
 </file>
@@ -557,7 +566,7 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>

</xml_diff>